<commit_message>
add back end e exemplo
</commit_message>
<xml_diff>
--- a/dc/cronograma_abril.xlsx
+++ b/dc/cronograma_abril.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robes\Desktop\tcc _ds\dc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA5CAB3-2C02-4CCD-BF9F-93920686DDD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9799CC98-59BA-4917-BC74-D9C95A857796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F1017B2-0076-4ACF-A0A4-7BCE96C889E5}"/>
   </bookViews>
@@ -540,6 +540,66 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -554,66 +614,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -982,7 +982,7 @@
   <dimension ref="B1:AP32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:F9"/>
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,253 +1024,253 @@
   <sheetData>
     <row r="1" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:42" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="61" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="59" t="s">
+      <c r="H2" s="61"/>
+      <c r="I2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="60"/>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="60"/>
-      <c r="AH2" s="60"/>
-      <c r="AI2" s="60"/>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="60"/>
-      <c r="AM2" s="60"/>
-      <c r="AN2" s="60"/>
-      <c r="AO2" s="61"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="45"/>
     </row>
     <row r="3" spans="2:42" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="56" t="s">
+      <c r="H3" s="49"/>
+      <c r="I3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57"/>
-      <c r="V3" s="57"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="57"/>
-      <c r="Z3" s="57"/>
-      <c r="AA3" s="57"/>
-      <c r="AB3" s="57"/>
-      <c r="AC3" s="57"/>
-      <c r="AD3" s="57"/>
-      <c r="AE3" s="57"/>
-      <c r="AF3" s="57"/>
-      <c r="AG3" s="57"/>
-      <c r="AH3" s="57"/>
-      <c r="AI3" s="57"/>
-      <c r="AJ3" s="57"/>
-      <c r="AK3" s="57"/>
-      <c r="AL3" s="57"/>
-      <c r="AM3" s="57"/>
-      <c r="AN3" s="57"/>
-      <c r="AO3" s="58"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="41"/>
+      <c r="AG3" s="41"/>
+      <c r="AH3" s="41"/>
+      <c r="AI3" s="41"/>
+      <c r="AJ3" s="41"/>
+      <c r="AK3" s="41"/>
+      <c r="AL3" s="41"/>
+      <c r="AM3" s="41"/>
+      <c r="AN3" s="41"/>
+      <c r="AO3" s="42"/>
     </row>
     <row r="4" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="56" t="s">
+      <c r="H4" s="49"/>
+      <c r="I4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="57"/>
-      <c r="AE4" s="57"/>
-      <c r="AF4" s="57"/>
-      <c r="AG4" s="57"/>
-      <c r="AH4" s="57"/>
-      <c r="AI4" s="57"/>
-      <c r="AJ4" s="57"/>
-      <c r="AK4" s="57"/>
-      <c r="AL4" s="57"/>
-      <c r="AM4" s="57"/>
-      <c r="AN4" s="57"/>
-      <c r="AO4" s="58"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="41"/>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="41"/>
+      <c r="AI4" s="41"/>
+      <c r="AJ4" s="41"/>
+      <c r="AK4" s="41"/>
+      <c r="AL4" s="41"/>
+      <c r="AM4" s="41"/>
+      <c r="AN4" s="41"/>
+      <c r="AO4" s="42"/>
     </row>
     <row r="5" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="56" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="57"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="57"/>
-      <c r="W5" s="57"/>
-      <c r="X5" s="57"/>
-      <c r="Y5" s="57"/>
-      <c r="Z5" s="57"/>
-      <c r="AA5" s="57"/>
-      <c r="AB5" s="57"/>
-      <c r="AC5" s="57"/>
-      <c r="AD5" s="57"/>
-      <c r="AE5" s="57"/>
-      <c r="AF5" s="57"/>
-      <c r="AG5" s="57"/>
-      <c r="AH5" s="57"/>
-      <c r="AI5" s="57"/>
-      <c r="AJ5" s="57"/>
-      <c r="AK5" s="57"/>
-      <c r="AL5" s="57"/>
-      <c r="AM5" s="57"/>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="58"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="41"/>
+      <c r="AB5" s="41"/>
+      <c r="AC5" s="41"/>
+      <c r="AD5" s="41"/>
+      <c r="AE5" s="41"/>
+      <c r="AF5" s="41"/>
+      <c r="AG5" s="41"/>
+      <c r="AH5" s="41"/>
+      <c r="AI5" s="41"/>
+      <c r="AJ5" s="41"/>
+      <c r="AK5" s="41"/>
+      <c r="AL5" s="41"/>
+      <c r="AM5" s="41"/>
+      <c r="AN5" s="41"/>
+      <c r="AO5" s="42"/>
     </row>
     <row r="6" spans="2:42" ht="21" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45" t="s">
+      <c r="F6" s="56"/>
+      <c r="G6" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="45"/>
+      <c r="H6" s="56"/>
       <c r="I6" s="48" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="48"/>
       <c r="K6" s="48"/>
-      <c r="L6" s="53" t="s">
+      <c r="L6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="54"/>
-      <c r="Z6" s="54"/>
-      <c r="AA6" s="54"/>
-      <c r="AB6" s="54"/>
-      <c r="AC6" s="54"/>
-      <c r="AD6" s="54"/>
-      <c r="AE6" s="54"/>
-      <c r="AF6" s="54"/>
-      <c r="AG6" s="54"/>
-      <c r="AH6" s="54"/>
-      <c r="AI6" s="54"/>
-      <c r="AJ6" s="54"/>
-      <c r="AK6" s="54"/>
-      <c r="AL6" s="54"/>
-      <c r="AM6" s="54"/>
-      <c r="AN6" s="54"/>
-      <c r="AO6" s="55"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="38"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="38"/>
+      <c r="AD6" s="38"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="38"/>
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="38"/>
+      <c r="AI6" s="38"/>
+      <c r="AJ6" s="38"/>
+      <c r="AK6" s="38"/>
+      <c r="AL6" s="38"/>
+      <c r="AM6" s="38"/>
+      <c r="AN6" s="38"/>
+      <c r="AO6" s="39"/>
     </row>
     <row r="7" spans="2:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1388,10 +1388,10 @@
       <c r="D8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="42"/>
+      <c r="F8" s="49"/>
       <c r="G8" s="9">
         <v>44284</v>
       </c>
@@ -1442,10 +1442,10 @@
       <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="42"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="9">
         <v>44284</v>
       </c>
@@ -1486,7 +1486,7 @@
       <c r="AN9" s="15"/>
       <c r="AO9" s="21"/>
     </row>
-    <row r="10" spans="2:42" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:42" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>3</v>
       </c>
@@ -1496,10 +1496,10 @@
       <c r="D10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="42"/>
+      <c r="F10" s="49"/>
       <c r="G10" s="14">
         <v>44285</v>
       </c>
@@ -1507,14 +1507,14 @@
         <v>44292</v>
       </c>
       <c r="I10" s="12"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
       <c r="R10" s="15"/>
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
@@ -1550,10 +1550,10 @@
       <c r="D11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="42"/>
+      <c r="F11" s="49"/>
       <c r="G11" s="14">
         <v>44285</v>
       </c>
@@ -1561,14 +1561,14 @@
         <v>44302</v>
       </c>
       <c r="I11" s="12"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
       <c r="R11" s="26"/>
       <c r="S11" s="26"/>
       <c r="T11" s="26"/>
@@ -1604,10 +1604,10 @@
       <c r="D12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="52"/>
+      <c r="F12" s="53"/>
       <c r="G12" s="14">
         <v>44285</v>
       </c>
@@ -1658,10 +1658,10 @@
       <c r="D13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="42"/>
+      <c r="F13" s="49"/>
       <c r="G13" s="9">
         <v>44256</v>
       </c>
@@ -1712,10 +1712,10 @@
       <c r="D14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="42"/>
+      <c r="F14" s="49"/>
       <c r="G14" s="9">
         <v>44260</v>
       </c>
@@ -1762,10 +1762,10 @@
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="33"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
@@ -1804,10 +1804,10 @@
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="29"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
@@ -1991,11 +1991,17 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="L6:AO6"/>
-    <mergeCell ref="I5:AO5"/>
-    <mergeCell ref="I4:AO4"/>
-    <mergeCell ref="I3:AO3"/>
-    <mergeCell ref="I2:AO2"/>
+    <mergeCell ref="B2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="I6:K6"/>
@@ -2010,17 +2016,11 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L6:AO6"/>
+    <mergeCell ref="I5:AO5"/>
+    <mergeCell ref="I4:AO4"/>
+    <mergeCell ref="I3:AO3"/>
+    <mergeCell ref="I2:AO2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
add back e exemplos de documentação
</commit_message>
<xml_diff>
--- a/dc/cronograma_abril.xlsx
+++ b/dc/cronograma_abril.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robes\Desktop\tcc _ds\dc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9799CC98-59BA-4917-BC74-D9C95A857796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3D2BB3-6970-42E0-BF14-46204ABFB4B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F1017B2-0076-4ACF-A0A4-7BCE96C889E5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Legenda</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Atrasado</t>
   </si>
   <si>
-    <t>Departamento: Senai jaguariúna-SP</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -75,15 +72,6 @@
     <t>ADM</t>
   </si>
   <si>
-    <t>DES</t>
-  </si>
-  <si>
-    <t>Revisão: 1.0</t>
-  </si>
-  <si>
-    <t>Data:  29/03/2021</t>
-  </si>
-  <si>
     <t>Supervisor: Robésio</t>
   </si>
   <si>
@@ -114,29 +102,44 @@
     <t>Desenvolver Layout  das Telas</t>
   </si>
   <si>
+    <t>Jenifer/Janderson</t>
+  </si>
+  <si>
+    <t>Robésio/Janderson/Ian</t>
+  </si>
+  <si>
+    <t>Acessar o Banco Através do JS</t>
+  </si>
+  <si>
+    <t>Desenvolver Documentação</t>
+  </si>
+  <si>
+    <t>Desenvolver Aplicativo</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>Robésio/Jenifer/Cristian</t>
+  </si>
+  <si>
+    <t>Revisão: 1.1</t>
+  </si>
+  <si>
+    <t>Data:  17/04/2021</t>
+  </si>
+  <si>
+    <t>Departamento: Senai jaguariúna - SP</t>
+  </si>
+  <si>
     <t>Maísa</t>
-  </si>
-  <si>
-    <t>Jenifer/Janderson</t>
-  </si>
-  <si>
-    <t>Robésio/Janderson/Ian</t>
-  </si>
-  <si>
-    <t>Acessar o Banco Através do JS</t>
-  </si>
-  <si>
-    <t>Desenvolver Documentação</t>
-  </si>
-  <si>
-    <t>Robésio/Jenifer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,12 +196,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -381,21 +378,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -458,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -507,7 +489,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -525,14 +506,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,33 +518,39 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -577,12 +561,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -982,7 +960,7 @@
   <dimension ref="B1:AP32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+      <selection activeCell="E14" sqref="E14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +969,7 @@
     <col min="2" max="2" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="8" width="15.5703125" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
@@ -1024,19 +1002,19 @@
   <sheetData>
     <row r="1" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:42" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="61" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="59" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="61" t="s">
+      <c r="G2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="61"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="43" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J2" s="44"/>
       <c r="K2" s="44"/>
@@ -1072,9 +1050,9 @@
       <c r="AO2" s="45"/>
     </row>
     <row r="3" spans="2:42" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="49"/>
       <c r="F3" s="2"/>
       <c r="G3" s="49" t="s">
@@ -1082,7 +1060,7 @@
       </c>
       <c r="H3" s="49"/>
       <c r="I3" s="40" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="J3" s="41"/>
       <c r="K3" s="41"/>
@@ -1118,9 +1096,9 @@
       <c r="AO3" s="42"/>
     </row>
     <row r="4" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="49"/>
       <c r="F4" s="3"/>
       <c r="G4" s="49" t="s">
@@ -1128,7 +1106,7 @@
       </c>
       <c r="H4" s="49"/>
       <c r="I4" s="40" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J4" s="41"/>
       <c r="K4" s="41"/>
@@ -1164,8 +1142,8 @@
       <c r="AO4" s="42"/>
     </row>
     <row r="5" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
-        <v>18</v>
+      <c r="B5" s="52" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="49"/>
       <c r="D5" s="49"/>
@@ -1174,7 +1152,7 @@
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
       <c r="I5" s="40" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="J5" s="41"/>
       <c r="K5" s="41"/>
@@ -1210,30 +1188,30 @@
       <c r="AO5" s="42"/>
     </row>
     <row r="6" spans="2:42" ht="21" x14ac:dyDescent="0.25">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="D6" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="E6" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="F6" s="54"/>
+      <c r="G6" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56" t="s">
+      <c r="H6" s="54"/>
+      <c r="I6" s="48" t="s">
         <v>9</v>
-      </c>
-      <c r="H6" s="56"/>
-      <c r="I6" s="48" t="s">
-        <v>10</v>
       </c>
       <c r="J6" s="48"/>
       <c r="K6" s="48"/>
       <c r="L6" s="37" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M6" s="38"/>
       <c r="N6" s="38"/>
@@ -1266,16 +1244,16 @@
       <c r="AO6" s="39"/>
     </row>
     <row r="7" spans="2:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
       <c r="G7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="I7" s="4">
         <v>29</v>
@@ -1373,23 +1351,23 @@
       <c r="AN7" s="4">
         <v>29</v>
       </c>
-      <c r="AO7" s="25">
+      <c r="AO7" s="24">
         <v>30</v>
       </c>
-      <c r="AP7" s="24"/>
+      <c r="AP7" s="23"/>
     </row>
     <row r="8" spans="2:42" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F8" s="49"/>
       <c r="G8" s="9">
@@ -1437,13 +1415,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F9" s="49"/>
       <c r="G9" s="9">
@@ -1491,13 +1469,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="E10" s="49" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F10" s="49"/>
       <c r="G10" s="14">
@@ -1540,25 +1518,25 @@
       <c r="AN10" s="15"/>
       <c r="AO10" s="21"/>
     </row>
-    <row r="11" spans="2:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>4</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F11" s="49"/>
       <c r="G11" s="14">
         <v>44285</v>
       </c>
       <c r="H11" s="14">
-        <v>44302</v>
+        <v>44305</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="10"/>
@@ -1569,19 +1547,19 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="15"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
       <c r="AE11" s="15"/>
       <c r="AF11" s="15"/>
       <c r="AG11" s="15"/>
@@ -1599,74 +1577,74 @@
         <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="53"/>
+        <v>22</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="51"/>
       <c r="G12" s="14">
         <v>44285</v>
       </c>
       <c r="H12" s="14">
-        <v>44288</v>
+        <v>44316</v>
       </c>
       <c r="I12" s="12"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="15"/>
-      <c r="AG12" s="15"/>
-      <c r="AH12" s="15"/>
-      <c r="AI12" s="15"/>
-      <c r="AJ12" s="15"/>
-      <c r="AK12" s="15"/>
-      <c r="AL12" s="15"/>
-      <c r="AM12" s="15"/>
-      <c r="AN12" s="15"/>
-      <c r="AO12" s="21"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="25"/>
+      <c r="AF12" s="25"/>
+      <c r="AG12" s="25"/>
+      <c r="AH12" s="25"/>
+      <c r="AI12" s="25"/>
+      <c r="AJ12" s="25"/>
+      <c r="AK12" s="25"/>
+      <c r="AL12" s="25"/>
+      <c r="AM12" s="25"/>
+      <c r="AN12" s="25"/>
+      <c r="AO12" s="25"/>
     </row>
     <row r="13" spans="2:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F13" s="49"/>
       <c r="G13" s="9">
-        <v>44256</v>
+        <v>44306</v>
       </c>
       <c r="H13" s="9">
-        <v>44259</v>
+        <v>44316</v>
       </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
@@ -1686,10 +1664,10 @@
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="20"/>
-      <c r="AC13" s="20"/>
-      <c r="AD13" s="20"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="12"/>
       <c r="AE13" s="20"/>
       <c r="AF13" s="20"/>
       <c r="AG13" s="20"/>
@@ -1700,20 +1678,20 @@
       <c r="AL13" s="20"/>
       <c r="AM13" s="20"/>
       <c r="AN13" s="20"/>
-      <c r="AO13" s="32"/>
+      <c r="AO13" s="31"/>
     </row>
     <row r="14" spans="2:42" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F14" s="49"/>
       <c r="G14" s="9">
@@ -1723,27 +1701,27 @@
         <v>44260</v>
       </c>
       <c r="I14" s="12"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="20"/>
-      <c r="W14" s="20"/>
-      <c r="X14" s="20"/>
-      <c r="Y14" s="20"/>
-      <c r="Z14" s="20"/>
-      <c r="AA14" s="20"/>
-      <c r="AB14" s="20"/>
-      <c r="AC14" s="20"/>
-      <c r="AD14" s="20"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="10"/>
       <c r="AE14" s="20"/>
       <c r="AF14" s="20"/>
       <c r="AG14" s="20"/>
@@ -1754,24 +1732,34 @@
       <c r="AL14" s="20"/>
       <c r="AM14" s="20"/>
       <c r="AN14" s="20"/>
-      <c r="AO14" s="32"/>
-    </row>
-    <row r="15" spans="2:42" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO14" s="31"/>
+    </row>
+    <row r="15" spans="2:42" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16">
         <v>8</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
+      <c r="C15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="49"/>
+      <c r="G15" s="36">
+        <v>44306</v>
+      </c>
+      <c r="H15" s="36">
+        <v>44316</v>
+      </c>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
-      <c r="L15" s="34"/>
+      <c r="L15" s="32"/>
       <c r="M15" s="19"/>
-      <c r="N15" s="35"/>
+      <c r="N15" s="33"/>
       <c r="O15" s="18"/>
       <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
@@ -1788,209 +1776,209 @@
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
       <c r="AD15" s="19"/>
-      <c r="AE15" s="19"/>
-      <c r="AF15" s="19"/>
-      <c r="AG15" s="19"/>
-      <c r="AH15" s="19"/>
-      <c r="AI15" s="19"/>
-      <c r="AJ15" s="19"/>
-      <c r="AK15" s="19"/>
-      <c r="AL15" s="19"/>
-      <c r="AM15" s="19"/>
-      <c r="AN15" s="19"/>
-      <c r="AO15" s="22"/>
+      <c r="AE15" s="20"/>
+      <c r="AF15" s="20"/>
+      <c r="AG15" s="20"/>
+      <c r="AH15" s="20"/>
+      <c r="AI15" s="20"/>
+      <c r="AJ15" s="20"/>
+      <c r="AK15" s="20"/>
+      <c r="AL15" s="20"/>
+      <c r="AM15" s="20"/>
+      <c r="AN15" s="20"/>
+      <c r="AO15" s="31"/>
     </row>
     <row r="16" spans="2:42" ht="18" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="23"/>
-      <c r="AF16" s="23"/>
-      <c r="AG16" s="23"/>
-      <c r="AH16" s="23"/>
-      <c r="AI16" s="23"/>
-      <c r="AJ16" s="23"/>
-      <c r="AK16" s="23"/>
-      <c r="AL16" s="23"/>
-      <c r="AM16" s="23"/>
-      <c r="AN16" s="23"/>
-      <c r="AO16" s="23"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="22"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="22"/>
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="22"/>
+      <c r="AD16" s="22"/>
+      <c r="AE16" s="22"/>
+      <c r="AF16" s="22"/>
+      <c r="AG16" s="22"/>
+      <c r="AH16" s="22"/>
+      <c r="AI16" s="22"/>
+      <c r="AJ16" s="22"/>
+      <c r="AK16" s="22"/>
+      <c r="AL16" s="22"/>
+      <c r="AM16" s="22"/>
+      <c r="AN16" s="22"/>
+      <c r="AO16" s="22"/>
     </row>
     <row r="17" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
-      <c r="AD17" s="23"/>
-      <c r="AE17" s="23"/>
-      <c r="AF17" s="23"/>
-      <c r="AG17" s="23"/>
-      <c r="AH17" s="23"/>
-      <c r="AI17" s="23"/>
-      <c r="AJ17" s="23"/>
-      <c r="AK17" s="23"/>
-      <c r="AL17" s="23"/>
-      <c r="AM17" s="23"/>
-      <c r="AN17" s="23"/>
-      <c r="AO17" s="23"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22"/>
+      <c r="AH17" s="22"/>
+      <c r="AI17" s="22"/>
+      <c r="AJ17" s="22"/>
+      <c r="AK17" s="22"/>
+      <c r="AL17" s="22"/>
+      <c r="AM17" s="22"/>
+      <c r="AN17" s="22"/>
+      <c r="AO17" s="22"/>
     </row>
     <row r="18" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="19" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
     </row>
     <row r="20" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
     </row>
     <row r="21" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="D21" s="23"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="46"/>
       <c r="F21" s="47"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="D22" s="23"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="46"/>
       <c r="F22" s="47"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
     </row>
     <row r="23" spans="2:41" ht="18" x14ac:dyDescent="0.25">
-      <c r="D23" s="23"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" spans="2:41" ht="18" x14ac:dyDescent="0.25">
-      <c r="D24" s="23"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
     </row>
     <row r="25" spans="2:41" ht="18" x14ac:dyDescent="0.25">
-      <c r="D25" s="23"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
     </row>
     <row r="26" spans="2:41" ht="18" x14ac:dyDescent="0.25">
-      <c r="D26" s="23"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
     </row>
     <row r="27" spans="2:41" ht="18" x14ac:dyDescent="0.25">
-      <c r="D27" s="23"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
     </row>
     <row r="28" spans="2:41" ht="18" x14ac:dyDescent="0.25">
-      <c r="D28" s="23"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
     </row>
     <row r="29" spans="2:41" ht="18" x14ac:dyDescent="0.25">
-      <c r="D29" s="23"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
     </row>
     <row r="30" spans="2:41" ht="18" x14ac:dyDescent="0.25">
-      <c r="D30" s="23"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
     </row>
     <row r="31" spans="2:41" ht="18" x14ac:dyDescent="0.25">
-      <c r="D31" s="23"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
     </row>
     <row r="32" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="29">
     <mergeCell ref="B2:D4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="G2:H2"/>
@@ -2008,7 +1996,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="E8:F8"/>

</xml_diff>

<commit_message>
tbalimentos não edita img
</commit_message>
<xml_diff>
--- a/dc/cronograma_abril.xlsx
+++ b/dc/cronograma_abril.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robes\Desktop\tcc _ds\dc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3D2BB3-6970-42E0-BF14-46204ABFB4B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E26A8DD-ACB1-4D08-BDF5-C545D4A64263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F1017B2-0076-4ACF-A0A4-7BCE96C889E5}"/>
   </bookViews>
@@ -440,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -524,6 +524,48 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -551,46 +593,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -960,7 +963,7 @@
   <dimension ref="B1:AP32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:F14"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,253 +1005,253 @@
   <sheetData>
     <row r="1" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:42" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="55"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="59" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="41" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="43" t="s">
+      <c r="H2" s="41"/>
+      <c r="I2" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AG2" s="44"/>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="45"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="59"/>
     </row>
     <row r="3" spans="2:42" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="49"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="49"/>
-      <c r="I3" s="40" t="s">
+      <c r="H3" s="42"/>
+      <c r="I3" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
-      <c r="X3" s="41"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="41"/>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="41"/>
-      <c r="AC3" s="41"/>
-      <c r="AD3" s="41"/>
-      <c r="AE3" s="41"/>
-      <c r="AF3" s="41"/>
-      <c r="AG3" s="41"/>
-      <c r="AH3" s="41"/>
-      <c r="AI3" s="41"/>
-      <c r="AJ3" s="41"/>
-      <c r="AK3" s="41"/>
-      <c r="AL3" s="41"/>
-      <c r="AM3" s="41"/>
-      <c r="AN3" s="41"/>
-      <c r="AO3" s="42"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="55"/>
+      <c r="W3" s="55"/>
+      <c r="X3" s="55"/>
+      <c r="Y3" s="55"/>
+      <c r="Z3" s="55"/>
+      <c r="AA3" s="55"/>
+      <c r="AB3" s="55"/>
+      <c r="AC3" s="55"/>
+      <c r="AD3" s="55"/>
+      <c r="AE3" s="55"/>
+      <c r="AF3" s="55"/>
+      <c r="AG3" s="55"/>
+      <c r="AH3" s="55"/>
+      <c r="AI3" s="55"/>
+      <c r="AJ3" s="55"/>
+      <c r="AK3" s="55"/>
+      <c r="AL3" s="55"/>
+      <c r="AM3" s="55"/>
+      <c r="AN3" s="55"/>
+      <c r="AO3" s="56"/>
     </row>
     <row r="4" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="57"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="49"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="49"/>
-      <c r="I4" s="40" t="s">
+      <c r="H4" s="42"/>
+      <c r="I4" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="41"/>
-      <c r="AA4" s="41"/>
-      <c r="AB4" s="41"/>
-      <c r="AC4" s="41"/>
-      <c r="AD4" s="41"/>
-      <c r="AE4" s="41"/>
-      <c r="AF4" s="41"/>
-      <c r="AG4" s="41"/>
-      <c r="AH4" s="41"/>
-      <c r="AI4" s="41"/>
-      <c r="AJ4" s="41"/>
-      <c r="AK4" s="41"/>
-      <c r="AL4" s="41"/>
-      <c r="AM4" s="41"/>
-      <c r="AN4" s="41"/>
-      <c r="AO4" s="42"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="55"/>
+      <c r="U4" s="55"/>
+      <c r="V4" s="55"/>
+      <c r="W4" s="55"/>
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="55"/>
+      <c r="AB4" s="55"/>
+      <c r="AC4" s="55"/>
+      <c r="AD4" s="55"/>
+      <c r="AE4" s="55"/>
+      <c r="AF4" s="55"/>
+      <c r="AG4" s="55"/>
+      <c r="AH4" s="55"/>
+      <c r="AI4" s="55"/>
+      <c r="AJ4" s="55"/>
+      <c r="AK4" s="55"/>
+      <c r="AL4" s="55"/>
+      <c r="AM4" s="55"/>
+      <c r="AN4" s="55"/>
+      <c r="AO4" s="56"/>
     </row>
     <row r="5" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="40" t="s">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="41"/>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="41"/>
-      <c r="AA5" s="41"/>
-      <c r="AB5" s="41"/>
-      <c r="AC5" s="41"/>
-      <c r="AD5" s="41"/>
-      <c r="AE5" s="41"/>
-      <c r="AF5" s="41"/>
-      <c r="AG5" s="41"/>
-      <c r="AH5" s="41"/>
-      <c r="AI5" s="41"/>
-      <c r="AJ5" s="41"/>
-      <c r="AK5" s="41"/>
-      <c r="AL5" s="41"/>
-      <c r="AM5" s="41"/>
-      <c r="AN5" s="41"/>
-      <c r="AO5" s="42"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="55"/>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="55"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="55"/>
+      <c r="X5" s="55"/>
+      <c r="Y5" s="55"/>
+      <c r="Z5" s="55"/>
+      <c r="AA5" s="55"/>
+      <c r="AB5" s="55"/>
+      <c r="AC5" s="55"/>
+      <c r="AD5" s="55"/>
+      <c r="AE5" s="55"/>
+      <c r="AF5" s="55"/>
+      <c r="AG5" s="55"/>
+      <c r="AH5" s="55"/>
+      <c r="AI5" s="55"/>
+      <c r="AJ5" s="55"/>
+      <c r="AK5" s="55"/>
+      <c r="AL5" s="55"/>
+      <c r="AM5" s="55"/>
+      <c r="AN5" s="55"/>
+      <c r="AO5" s="56"/>
     </row>
     <row r="6" spans="2:42" ht="21" x14ac:dyDescent="0.25">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54" t="s">
+      <c r="F6" s="45"/>
+      <c r="G6" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="54"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="48" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="48"/>
       <c r="K6" s="48"/>
-      <c r="L6" s="37" t="s">
+      <c r="L6" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="38"/>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="38"/>
-      <c r="AB6" s="38"/>
-      <c r="AC6" s="38"/>
-      <c r="AD6" s="38"/>
-      <c r="AE6" s="38"/>
-      <c r="AF6" s="38"/>
-      <c r="AG6" s="38"/>
-      <c r="AH6" s="38"/>
-      <c r="AI6" s="38"/>
-      <c r="AJ6" s="38"/>
-      <c r="AK6" s="38"/>
-      <c r="AL6" s="38"/>
-      <c r="AM6" s="38"/>
-      <c r="AN6" s="38"/>
-      <c r="AO6" s="39"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="52"/>
+      <c r="S6" s="52"/>
+      <c r="T6" s="52"/>
+      <c r="U6" s="52"/>
+      <c r="V6" s="52"/>
+      <c r="W6" s="52"/>
+      <c r="X6" s="52"/>
+      <c r="Y6" s="52"/>
+      <c r="Z6" s="52"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="52"/>
+      <c r="AC6" s="52"/>
+      <c r="AD6" s="52"/>
+      <c r="AE6" s="52"/>
+      <c r="AF6" s="52"/>
+      <c r="AG6" s="52"/>
+      <c r="AH6" s="52"/>
+      <c r="AI6" s="52"/>
+      <c r="AJ6" s="52"/>
+      <c r="AK6" s="52"/>
+      <c r="AL6" s="52"/>
+      <c r="AM6" s="52"/>
+      <c r="AN6" s="52"/>
+      <c r="AO6" s="53"/>
     </row>
     <row r="7" spans="2:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="53"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
       <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1366,10 +1369,10 @@
       <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="49"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="9">
         <v>44284</v>
       </c>
@@ -1420,10 +1423,10 @@
       <c r="D9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="49"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="9">
         <v>44284</v>
       </c>
@@ -1474,10 +1477,10 @@
       <c r="D10" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="49"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="14">
         <v>44285</v>
       </c>
@@ -1528,10 +1531,10 @@
       <c r="D11" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="49"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="14">
         <v>44285</v>
       </c>
@@ -1582,10 +1585,10 @@
       <c r="D12" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="51"/>
+      <c r="F12" s="50"/>
       <c r="G12" s="14">
         <v>44285</v>
       </c>
@@ -1636,10 +1639,10 @@
       <c r="D13" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="49"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="9">
         <v>44306</v>
       </c>
@@ -1690,10 +1693,10 @@
       <c r="D14" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E14" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="49"/>
+      <c r="F14" s="42"/>
       <c r="G14" s="9">
         <v>44260</v>
       </c>
@@ -1701,22 +1704,22 @@
         <v>44260</v>
       </c>
       <c r="I14" s="12"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
+      <c r="T14" s="60"/>
+      <c r="U14" s="60"/>
+      <c r="V14" s="60"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="60"/>
+      <c r="Y14" s="60"/>
       <c r="Z14" s="10"/>
       <c r="AA14" s="10"/>
       <c r="AB14" s="10"/>
@@ -1744,10 +1747,10 @@
       <c r="D15" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="E15" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="49"/>
+      <c r="F15" s="42"/>
       <c r="G15" s="36">
         <v>44306</v>
       </c>
@@ -1792,10 +1795,10 @@
       <c r="B16" s="26"/>
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
@@ -1979,17 +1982,11 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="L6:AO6"/>
+    <mergeCell ref="I5:AO5"/>
+    <mergeCell ref="I4:AO4"/>
+    <mergeCell ref="I3:AO3"/>
+    <mergeCell ref="I2:AO2"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="I6:K6"/>
@@ -2003,11 +2000,17 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="L6:AO6"/>
-    <mergeCell ref="I5:AO5"/>
-    <mergeCell ref="I4:AO4"/>
-    <mergeCell ref="I3:AO3"/>
-    <mergeCell ref="I2:AO2"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
banco de dados atualizado
</commit_message>
<xml_diff>
--- a/dc/cronograma_abril.xlsx
+++ b/dc/cronograma_abril.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robes\Desktop\tcc _ds\dc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E26A8DD-ACB1-4D08-BDF5-C545D4A64263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9CDE2C-1BA6-412B-9627-CB5484A68CDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F1017B2-0076-4ACF-A0A4-7BCE96C889E5}"/>
   </bookViews>
@@ -123,16 +123,16 @@
     <t>Robésio/Jenifer/Cristian</t>
   </si>
   <si>
-    <t>Revisão: 1.1</t>
-  </si>
-  <si>
-    <t>Data:  17/04/2021</t>
-  </si>
-  <si>
     <t>Departamento: Senai jaguariúna - SP</t>
   </si>
   <si>
     <t>Maísa</t>
+  </si>
+  <si>
+    <t>Data:  26/04/2021</t>
+  </si>
+  <si>
+    <t>Revisão: 1.3</t>
   </si>
 </sst>
 </file>
@@ -524,6 +524,63 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -537,63 +594,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -963,7 +963,7 @@
   <dimension ref="B1:AP32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+      <selection activeCell="I3" sqref="I3:AO3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,253 +1005,253 @@
   <sheetData>
     <row r="1" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:42" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="60" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="60"/>
+      <c r="I2" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="45"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="45"/>
+      <c r="AL2" s="45"/>
+      <c r="AM2" s="45"/>
+      <c r="AN2" s="45"/>
+      <c r="AO2" s="46"/>
+    </row>
+    <row r="3" spans="2:42" ht="18" x14ac:dyDescent="0.25">
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="50"/>
+      <c r="I3" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="42"/>
+      <c r="V3" s="42"/>
+      <c r="W3" s="42"/>
+      <c r="X3" s="42"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="42"/>
+      <c r="AA3" s="42"/>
+      <c r="AB3" s="42"/>
+      <c r="AC3" s="42"/>
+      <c r="AD3" s="42"/>
+      <c r="AE3" s="42"/>
+      <c r="AF3" s="42"/>
+      <c r="AG3" s="42"/>
+      <c r="AH3" s="42"/>
+      <c r="AI3" s="42"/>
+      <c r="AJ3" s="42"/>
+      <c r="AK3" s="42"/>
+      <c r="AL3" s="42"/>
+      <c r="AM3" s="42"/>
+      <c r="AN3" s="42"/>
+      <c r="AO3" s="43"/>
+    </row>
+    <row r="4" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="50"/>
+      <c r="I4" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
+      <c r="AA4" s="42"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="42"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="42"/>
+      <c r="AF4" s="42"/>
+      <c r="AG4" s="42"/>
+      <c r="AH4" s="42"/>
+      <c r="AI4" s="42"/>
+      <c r="AJ4" s="42"/>
+      <c r="AK4" s="42"/>
+      <c r="AL4" s="42"/>
+      <c r="AM4" s="42"/>
+      <c r="AN4" s="42"/>
+      <c r="AO4" s="43"/>
+    </row>
+    <row r="5" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="58"/>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="58"/>
-      <c r="AC2" s="58"/>
-      <c r="AD2" s="58"/>
-      <c r="AE2" s="58"/>
-      <c r="AF2" s="58"/>
-      <c r="AG2" s="58"/>
-      <c r="AH2" s="58"/>
-      <c r="AI2" s="58"/>
-      <c r="AJ2" s="58"/>
-      <c r="AK2" s="58"/>
-      <c r="AL2" s="58"/>
-      <c r="AM2" s="58"/>
-      <c r="AN2" s="58"/>
-      <c r="AO2" s="59"/>
-    </row>
-    <row r="3" spans="2:42" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="55"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="55"/>
-      <c r="AA3" s="55"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="55"/>
-      <c r="AE3" s="55"/>
-      <c r="AF3" s="55"/>
-      <c r="AG3" s="55"/>
-      <c r="AH3" s="55"/>
-      <c r="AI3" s="55"/>
-      <c r="AJ3" s="55"/>
-      <c r="AK3" s="55"/>
-      <c r="AL3" s="55"/>
-      <c r="AM3" s="55"/>
-      <c r="AN3" s="55"/>
-      <c r="AO3" s="56"/>
-    </row>
-    <row r="4" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
-      <c r="U4" s="55"/>
-      <c r="V4" s="55"/>
-      <c r="W4" s="55"/>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="55"/>
-      <c r="AB4" s="55"/>
-      <c r="AC4" s="55"/>
-      <c r="AD4" s="55"/>
-      <c r="AE4" s="55"/>
-      <c r="AF4" s="55"/>
-      <c r="AG4" s="55"/>
-      <c r="AH4" s="55"/>
-      <c r="AI4" s="55"/>
-      <c r="AJ4" s="55"/>
-      <c r="AK4" s="55"/>
-      <c r="AL4" s="55"/>
-      <c r="AM4" s="55"/>
-      <c r="AN4" s="55"/>
-      <c r="AO4" s="56"/>
-    </row>
-    <row r="5" spans="2:42" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="55"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="55"/>
-      <c r="V5" s="55"/>
-      <c r="W5" s="55"/>
-      <c r="X5" s="55"/>
-      <c r="Y5" s="55"/>
-      <c r="Z5" s="55"/>
-      <c r="AA5" s="55"/>
-      <c r="AB5" s="55"/>
-      <c r="AC5" s="55"/>
-      <c r="AD5" s="55"/>
-      <c r="AE5" s="55"/>
-      <c r="AF5" s="55"/>
-      <c r="AG5" s="55"/>
-      <c r="AH5" s="55"/>
-      <c r="AI5" s="55"/>
-      <c r="AJ5" s="55"/>
-      <c r="AK5" s="55"/>
-      <c r="AL5" s="55"/>
-      <c r="AM5" s="55"/>
-      <c r="AN5" s="55"/>
-      <c r="AO5" s="56"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="42"/>
+      <c r="X5" s="42"/>
+      <c r="Y5" s="42"/>
+      <c r="Z5" s="42"/>
+      <c r="AA5" s="42"/>
+      <c r="AB5" s="42"/>
+      <c r="AC5" s="42"/>
+      <c r="AD5" s="42"/>
+      <c r="AE5" s="42"/>
+      <c r="AF5" s="42"/>
+      <c r="AG5" s="42"/>
+      <c r="AH5" s="42"/>
+      <c r="AI5" s="42"/>
+      <c r="AJ5" s="42"/>
+      <c r="AK5" s="42"/>
+      <c r="AL5" s="42"/>
+      <c r="AM5" s="42"/>
+      <c r="AN5" s="42"/>
+      <c r="AO5" s="43"/>
     </row>
     <row r="6" spans="2:42" ht="21" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45" t="s">
+      <c r="F6" s="55"/>
+      <c r="G6" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="45"/>
-      <c r="I6" s="48" t="s">
+      <c r="H6" s="55"/>
+      <c r="I6" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="51" t="s">
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="52"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="52"/>
-      <c r="Z6" s="52"/>
-      <c r="AA6" s="52"/>
-      <c r="AB6" s="52"/>
-      <c r="AC6" s="52"/>
-      <c r="AD6" s="52"/>
-      <c r="AE6" s="52"/>
-      <c r="AF6" s="52"/>
-      <c r="AG6" s="52"/>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="52"/>
-      <c r="AJ6" s="52"/>
-      <c r="AK6" s="52"/>
-      <c r="AL6" s="52"/>
-      <c r="AM6" s="52"/>
-      <c r="AN6" s="52"/>
-      <c r="AO6" s="53"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="39"/>
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="39"/>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="39"/>
+      <c r="AG6" s="39"/>
+      <c r="AH6" s="39"/>
+      <c r="AI6" s="39"/>
+      <c r="AJ6" s="39"/>
+      <c r="AK6" s="39"/>
+      <c r="AL6" s="39"/>
+      <c r="AM6" s="39"/>
+      <c r="AN6" s="39"/>
+      <c r="AO6" s="40"/>
     </row>
     <row r="7" spans="2:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
       <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1369,10 +1369,10 @@
       <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="42"/>
+      <c r="F8" s="50"/>
       <c r="G8" s="9">
         <v>44284</v>
       </c>
@@ -1423,10 +1423,10 @@
       <c r="D9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="42"/>
+      <c r="F9" s="50"/>
       <c r="G9" s="9">
         <v>44284</v>
       </c>
@@ -1477,10 +1477,10 @@
       <c r="D10" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="42"/>
+      <c r="F10" s="50"/>
       <c r="G10" s="14">
         <v>44285</v>
       </c>
@@ -1531,10 +1531,10 @@
       <c r="D11" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="42"/>
+      <c r="F11" s="50"/>
       <c r="G11" s="14">
         <v>44285</v>
       </c>
@@ -1585,10 +1585,10 @@
       <c r="D12" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="50"/>
+      <c r="E12" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="52"/>
       <c r="G12" s="14">
         <v>44285</v>
       </c>
@@ -1617,13 +1617,13 @@
       <c r="AB12" s="10"/>
       <c r="AC12" s="10"/>
       <c r="AD12" s="10"/>
-      <c r="AE12" s="25"/>
-      <c r="AF12" s="25"/>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="25"/>
-      <c r="AI12" s="25"/>
-      <c r="AJ12" s="25"/>
-      <c r="AK12" s="25"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="10"/>
+      <c r="AJ12" s="10"/>
+      <c r="AK12" s="10"/>
       <c r="AL12" s="25"/>
       <c r="AM12" s="25"/>
       <c r="AN12" s="25"/>
@@ -1639,10 +1639,10 @@
       <c r="D13" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="42"/>
+      <c r="F13" s="50"/>
       <c r="G13" s="9">
         <v>44306</v>
       </c>
@@ -1671,13 +1671,13 @@
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
       <c r="AD13" s="12"/>
-      <c r="AE13" s="20"/>
-      <c r="AF13" s="20"/>
-      <c r="AG13" s="20"/>
-      <c r="AH13" s="20"/>
-      <c r="AI13" s="20"/>
-      <c r="AJ13" s="20"/>
-      <c r="AK13" s="20"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+      <c r="AH13" s="10"/>
+      <c r="AI13" s="10"/>
+      <c r="AJ13" s="10"/>
+      <c r="AK13" s="10"/>
       <c r="AL13" s="20"/>
       <c r="AM13" s="20"/>
       <c r="AN13" s="20"/>
@@ -1693,10 +1693,10 @@
       <c r="D14" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="42"/>
+      <c r="F14" s="50"/>
       <c r="G14" s="9">
         <v>44260</v>
       </c>
@@ -1704,33 +1704,33 @@
         <v>44260</v>
       </c>
       <c r="I14" s="12"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="60"/>
-      <c r="U14" s="60"/>
-      <c r="V14" s="60"/>
-      <c r="W14" s="60"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="60"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="37"/>
       <c r="Z14" s="10"/>
       <c r="AA14" s="10"/>
       <c r="AB14" s="10"/>
       <c r="AC14" s="10"/>
       <c r="AD14" s="10"/>
-      <c r="AE14" s="20"/>
-      <c r="AF14" s="20"/>
-      <c r="AG14" s="20"/>
-      <c r="AH14" s="20"/>
-      <c r="AI14" s="20"/>
-      <c r="AJ14" s="20"/>
+      <c r="AE14" s="37"/>
+      <c r="AF14" s="37"/>
+      <c r="AG14" s="37"/>
+      <c r="AH14" s="37"/>
+      <c r="AI14" s="37"/>
+      <c r="AJ14" s="37"/>
       <c r="AK14" s="20"/>
       <c r="AL14" s="20"/>
       <c r="AM14" s="20"/>
@@ -1747,10 +1747,10 @@
       <c r="D15" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="42"/>
+      <c r="E15" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="50"/>
       <c r="G15" s="36">
         <v>44306</v>
       </c>
@@ -1795,10 +1795,10 @@
       <c r="B16" s="26"/>
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
@@ -1898,15 +1898,15 @@
     </row>
     <row r="21" spans="2:41" x14ac:dyDescent="0.25">
       <c r="D21" s="22"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="48"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
     </row>
     <row r="22" spans="2:41" x14ac:dyDescent="0.25">
       <c r="D22" s="22"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="48"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
     </row>
@@ -1982,11 +1982,17 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="L6:AO6"/>
-    <mergeCell ref="I5:AO5"/>
-    <mergeCell ref="I4:AO4"/>
-    <mergeCell ref="I3:AO3"/>
-    <mergeCell ref="I2:AO2"/>
+    <mergeCell ref="B2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="I6:K6"/>
@@ -2000,17 +2006,11 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L6:AO6"/>
+    <mergeCell ref="I5:AO5"/>
+    <mergeCell ref="I4:AO4"/>
+    <mergeCell ref="I3:AO3"/>
+    <mergeCell ref="I2:AO2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>